<commit_message>
fix: refatora motor de datas no comparativo anual para o formato do backend
</commit_message>
<xml_diff>
--- a/database/lojas e senhas.xlsx
+++ b/database/lojas e senhas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TeleFluxo_Instalador\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735217EA-E6ED-442F-B6E3-BAFE30E36784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207F16B9-A69C-4234-933C-98C8B29E9B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DC387A1A-0365-4EFE-8541-627FD66421E4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
   <si>
     <t>OPERAÇÃO</t>
   </si>
@@ -59,226 +59,238 @@
     <t>ARAGUAIA SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG ARAGUAIA SHOPPING</t>
-  </si>
-  <si>
     <t>samsungaraguaia@gmail.com</t>
   </si>
   <si>
     <t>BOULEVARD SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG BOULEVARD SHOPPING</t>
-  </si>
-  <si>
     <t>samsungboulevardqq@gmail.com</t>
   </si>
   <si>
     <t>BRASILIA SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG BRASILIA SHOPPING</t>
-  </si>
-  <si>
     <t>samsungbsbshopping@gmail.com</t>
   </si>
   <si>
     <t>CONJUNTO NACIONAL</t>
   </si>
   <si>
-    <t>SAMSUNG CONJUNTO NACIONAL</t>
-  </si>
-  <si>
     <t>samsung.cnb.2013@gmail.com</t>
   </si>
   <si>
     <t>CONJUNTO NACIONAL QUIOSQUE</t>
   </si>
   <si>
-    <t>SAMSUNG CONJUNTO NACIONAL QUIOSQUE</t>
-  </si>
-  <si>
     <t>quiosquesamsungcnb@gmail.com</t>
   </si>
   <si>
     <t>GOIANIA SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG GOIANIA SHOPPING</t>
-  </si>
-  <si>
     <t>lojasamsunggoianiashopping@gmail.com</t>
   </si>
   <si>
     <t>IGUATEMI SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG IGUATEMI SHOPPING</t>
-  </si>
-  <si>
     <t>iguatemisamsung@gmail.com</t>
   </si>
   <si>
     <t>JK SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG JK SHOPPING</t>
-  </si>
-  <si>
     <t>samsungjkshopping1@gmail.com</t>
   </si>
   <si>
     <t>PARK SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG PARK SHOPPING</t>
-  </si>
-  <si>
     <t>lojasamsungparkshopping@gmail.com</t>
   </si>
   <si>
     <t>PATIO BRASIL</t>
   </si>
   <si>
-    <t>SAMSUNG PATIO BRASIL</t>
-  </si>
-  <si>
     <t>samsungpatiobrasil@gmail.com</t>
   </si>
   <si>
     <t>TAGUATINGA SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG TAGUATINGA SHOPPING</t>
-  </si>
-  <si>
     <t>samsungtaguatingashopping@gmail.com</t>
   </si>
   <si>
     <t>TERRAÇO SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG TERRAÇO SHOPPING</t>
-  </si>
-  <si>
     <t>samsungterraco@gmail.com</t>
   </si>
   <si>
     <t>TAGUATINGA SHOPPING QQ</t>
   </si>
   <si>
-    <t>SAMSUNG TAGUATINGA SHOPPING QQ</t>
-  </si>
-  <si>
     <t>samsungqqtaguatinga.telecel@gmail.com</t>
   </si>
   <si>
     <t>UBERLÂNDIA SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG UBERLÂNDIA SHOPPING</t>
-  </si>
-  <si>
     <t>samsunguberlandia.telecel@gmail.com</t>
   </si>
   <si>
     <t>UBERABA SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG UBERABA SHOPPING</t>
-  </si>
-  <si>
     <t>samsunguberaba.telecel@gmail.com</t>
   </si>
   <si>
     <t>FLAMBOYANT SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG FLAMBOYANT SHOPPING</t>
-  </si>
-  <si>
     <t>flamboyantsamsung.telecel@gmail.com</t>
   </si>
   <si>
     <t>BURITI SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG BURITI SHOPPING</t>
-  </si>
-  <si>
     <t>samsungburitishopping.telecel@gmail.com</t>
   </si>
   <si>
     <t>PASSEIO DAS AGUAS</t>
   </si>
   <si>
-    <t>SAMSUNG PASSEIO DAS AGUAS</t>
-  </si>
-  <si>
     <t>samsungpasseio.telecel@gmail.com</t>
   </si>
   <si>
     <t>PORTAL SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG PORTAL SHOPPING</t>
-  </si>
-  <si>
     <t>samsungportalnorte.telecel@gmail.com</t>
   </si>
   <si>
     <t>SHOPPING SUL</t>
   </si>
   <si>
-    <t>SAMSUNG SHOPPING SUL</t>
-  </si>
-  <si>
     <t>samsungshoppingsul.telecel@gmail.com</t>
   </si>
   <si>
     <t>BURITI RIO VERDE</t>
   </si>
   <si>
-    <t>SAMSUNG BURITI RIO VERDE</t>
-  </si>
-  <si>
     <t>samsungrioverde.telecel@gmail.com</t>
   </si>
   <si>
     <t>PARK ANAPOLIS</t>
   </si>
   <si>
-    <t>SAMSUNG PARK ANAPOLIS</t>
-  </si>
-  <si>
     <t>samsungbraasilpark.telecel@gmail.com</t>
   </si>
   <si>
     <t>SHOPPING RECIFE</t>
   </si>
   <si>
-    <t>SAMSUNG SHOPPING RECIFE</t>
-  </si>
-  <si>
     <t xml:space="preserve">samsungrecife.telecel@gmail.com </t>
   </si>
   <si>
     <t>MANAIRA SHOPPING</t>
   </si>
   <si>
-    <t>SAMSUNG MANAIRA SHOPPING</t>
-  </si>
-  <si>
     <t>samsungmanaira.telecel@gmail.com</t>
   </si>
   <si>
     <t>IGUATEMI FORTALEZA</t>
   </si>
   <si>
-    <t>SAMSUNG IGUATEMI FORTALEZA</t>
-  </si>
-  <si>
     <t>samiguatemifortaleza.telecel@gmail.com</t>
+  </si>
+  <si>
+    <t>SSG ARAGUAIA SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG BOULEVARD SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG BRASILIA SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG CONJUNTO NACIONAL</t>
+  </si>
+  <si>
+    <t>SSG CONJUNTO NACIONAL QUIOSQUE</t>
+  </si>
+  <si>
+    <t>SSG GOIANIA SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG IGUATEMI SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG JK SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG PARK SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG PATIO BRASIL</t>
+  </si>
+  <si>
+    <t>SSG TAGUATINGA SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG TERRAÇO SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG TAGUATINGA SHOPPING QQ</t>
+  </si>
+  <si>
+    <t>SSG UBERLÂNDIA SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG UBERABA SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG FLAMBOYANT SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG BURITI SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG PASSEIO DAS AGUAS</t>
+  </si>
+  <si>
+    <t>SSG PORTAL SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG SHOPPING SUL</t>
+  </si>
+  <si>
+    <t>SSG BURITI RIO VERDE</t>
+  </si>
+  <si>
+    <t>SSG PARK ANAPOLIS</t>
+  </si>
+  <si>
+    <t>SSG SHOPPING RECIFE</t>
+  </si>
+  <si>
+    <t>SSG MANAIRA SHOPPING</t>
+  </si>
+  <si>
+    <t>SSG IGUATEMI FORTALEZA</t>
+  </si>
+  <si>
+    <t>LOJAS</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>GERENTE</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -320,7 +332,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,8 +345,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -357,12 +375,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,6 +409,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -678,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5622E-29A2-43BB-87B8-5D1BD5310F6A}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,11 +740,12 @@
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -709,460 +761,523 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="3">
         <v>14050</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>24050</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>58</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E4" s="3">
         <v>34050</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>59</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E5" s="3">
         <v>44050</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E6" s="3">
         <v>54050</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>61</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E7" s="3">
         <v>64050</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>62</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="E8" s="3">
         <v>74050</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>63</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="3">
         <v>84050</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>64</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="E10" s="3">
         <v>94050</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>33</v>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>65</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="E11" s="3">
         <v>104050</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>36</v>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="E12" s="3">
         <v>114050</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>39</v>
+      <c r="B13" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E13" s="3">
         <v>124050</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>42</v>
+      <c r="B14" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E14" s="3">
         <v>134050</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>45</v>
+      <c r="B15" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>47</v>
+        <v>69</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E15" s="3">
         <v>144050</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>48</v>
+      <c r="B16" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>50</v>
+        <v>70</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="E16" s="3">
         <v>154050</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>51</v>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>53</v>
+        <v>71</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="E17" s="3">
         <v>164050</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>54</v>
+      <c r="B18" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>56</v>
+        <v>72</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="E18" s="3">
         <v>174050</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>57</v>
+      <c r="B19" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>59</v>
+        <v>73</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="E19" s="3">
         <v>184050</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>60</v>
+      <c r="B20" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>62</v>
+        <v>74</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="E20" s="3">
         <v>194050</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>63</v>
+      <c r="B21" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="E21" s="3">
         <v>204050</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>66</v>
+      <c r="B22" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="E22" s="3">
         <v>214050</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>69</v>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="E23" s="3">
         <v>224050</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>72</v>
+      <c r="B24" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="E24" s="3">
         <v>234050</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="E25" s="3">
         <v>244050</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>78</v>
+      <c r="B26" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="3" t="s">
         <v>80</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="E26" s="3">
         <v>254050</v>
       </c>
+      <c r="F26" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{C1C54683-072A-42FC-A4E7-D1750D35D9C9}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{6A7D1175-F661-46A1-9880-81A34C79A8A1}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{C552F76C-A92B-45AD-ADCF-416317336C72}"/>
-    <hyperlink ref="D4" r:id="rId4" xr:uid="{F46AFB18-9D5E-4245-8E76-2C8A6BF41D86}"/>
-    <hyperlink ref="D7" r:id="rId5" display="loja.samsunggoiania@gmail.com" xr:uid="{21389D6F-D7FA-4CC3-AF3A-1063548B6A1E}"/>
-    <hyperlink ref="D11" r:id="rId6" xr:uid="{39067688-DFB0-4372-938F-13EDE645E3A5}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{0179511F-6217-4D32-B779-1D6919543BF6}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{9CA58024-E0DA-46EA-B484-BAFBC8FD88F2}"/>
-    <hyperlink ref="D12" r:id="rId9" xr:uid="{58B952E0-2738-43F4-A961-13E31525D2C2}"/>
-    <hyperlink ref="D13" r:id="rId10" xr:uid="{921A7D32-9980-4D2C-B69C-95B410676016}"/>
-    <hyperlink ref="D6" r:id="rId11" xr:uid="{C675B752-0D04-46C2-9997-BF50E577950F}"/>
-    <hyperlink ref="D2" r:id="rId12" xr:uid="{85FE57D1-7C8E-4F8B-98D4-236B3C7A873F}"/>
-    <hyperlink ref="D15" r:id="rId13" xr:uid="{E47F61A9-8F09-4BE3-91CA-F8072D5B8206}"/>
-    <hyperlink ref="D14" r:id="rId14" xr:uid="{BE5DD8A1-AB06-4EDB-94AC-A4CD15F2AF3C}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{DE7656AE-B4E1-4D35-842A-CDFF4D16D770}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{6BE1F920-675D-4620-9388-6604248B8F6A}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{4FB79E7E-B187-4968-97E4-3586897F1C95}"/>
-    <hyperlink ref="D19" r:id="rId18" xr:uid="{D219E1DB-61FB-4A4D-A800-9BF12B0E1599}"/>
-    <hyperlink ref="D20" r:id="rId19" xr:uid="{995FC513-6D7F-4C2B-A337-E933E8B37780}"/>
-    <hyperlink ref="D21" r:id="rId20" xr:uid="{B5ACCEE9-39D9-4D90-9ED8-7A2CB216ECDF}"/>
-    <hyperlink ref="D22" r:id="rId21" xr:uid="{0B4BD527-E5F4-43F0-80B1-7B62539DF1DE}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{AFAECB5F-6457-43E8-95EC-3D334F8F2411}"/>
-    <hyperlink ref="D24" r:id="rId23" xr:uid="{7F91AA7E-FB11-4EB3-9C6A-99834B4ECCA0}"/>
-    <hyperlink ref="D26" r:id="rId24" xr:uid="{9DEE462D-6C92-4031-93AF-C48DC650B834}"/>
-    <hyperlink ref="D25" r:id="rId25" xr:uid="{8A7F641B-0036-46C7-8A37-00EBC9722092}"/>
-  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: adiciona suporte a IMEI no Prisma e atualiza script de extracao de estoque
</commit_message>
<xml_diff>
--- a/database/lojas e senhas.xlsx
+++ b/database/lojas e senhas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TeleFluxo_Instalador\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207F16B9-A69C-4234-933C-98C8B29E9B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DC2AF5-A82C-4664-AF31-70B2036EFADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DC387A1A-0365-4EFE-8541-627FD66421E4}"/>
+    <workbookView xWindow="6360" yWindow="2235" windowWidth="21600" windowHeight="11295" xr2:uid="{DC387A1A-0365-4EFE-8541-627FD66421E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha4" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
   <si>
     <t>OPERAÇÃO</t>
   </si>
@@ -414,16 +414,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5622E-29A2-43BB-87B8-5D1BD5310F6A}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,10 +761,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>83</v>
       </c>
     </row>
@@ -778,13 +778,13 @@
       <c r="C2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="3">
         <v>14050</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -798,13 +798,13 @@
       <c r="C3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="3">
         <v>24050</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -818,14 +818,17 @@
       <c r="C4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3">
         <v>34050</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>81</v>
+      <c r="F4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -838,13 +841,13 @@
       <c r="C5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="3">
         <v>44050</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -858,13 +861,13 @@
       <c r="C6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="3">
         <v>54050</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -878,13 +881,13 @@
       <c r="C7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="3">
         <v>64050</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -898,13 +901,13 @@
       <c r="C8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="3">
         <v>74050</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -918,13 +921,13 @@
       <c r="C9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="3">
         <v>84050</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -938,13 +941,13 @@
       <c r="C10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="3">
         <v>94050</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -958,16 +961,16 @@
       <c r="C11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="3">
         <v>104050</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="8" t="s">
+      <c r="F11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>84</v>
       </c>
     </row>
@@ -981,13 +984,13 @@
       <c r="C12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="3">
         <v>114050</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1001,13 +1004,13 @@
       <c r="C13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="3">
         <v>124050</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1021,13 +1024,13 @@
       <c r="C14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="3">
         <v>134050</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1041,13 +1044,13 @@
       <c r="C15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="3">
         <v>144050</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1061,13 +1064,13 @@
       <c r="C16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="3">
         <v>154050</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1081,13 +1084,13 @@
       <c r="C17" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="3">
         <v>164050</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1101,13 +1104,13 @@
       <c r="C18" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="3">
         <v>174050</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1121,13 +1124,13 @@
       <c r="C19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" t="s">
         <v>41</v>
       </c>
       <c r="E19" s="3">
         <v>184050</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1141,16 +1144,16 @@
       <c r="C20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="3">
         <v>194050</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H20" s="8" t="s">
+      <c r="F20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1164,16 +1167,16 @@
       <c r="C21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="3">
         <v>204050</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21" s="8" t="s">
+      <c r="F21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1187,13 +1190,13 @@
       <c r="C22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="3">
         <v>214050</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1207,13 +1210,13 @@
       <c r="C23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="3">
         <v>224050</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1227,13 +1230,13 @@
       <c r="C24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" t="s">
         <v>51</v>
       </c>
       <c r="E24" s="3">
         <v>234050</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1247,13 +1250,13 @@
       <c r="C25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="3">
         <v>244050</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1267,13 +1270,13 @@
       <c r="C26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" t="s">
         <v>55</v>
       </c>
       <c r="E26" s="3">
         <v>254050</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correção dos filtros de categoria no SalesDashboard, ajuste de devoluções no Python e atualização do Banco de Dados
</commit_message>
<xml_diff>
--- a/database/lojas e senhas.xlsx
+++ b/database/lojas e senhas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TeleFluxo_Instalador\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DC2AF5-A82C-4664-AF31-70B2036EFADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E5C17-73E3-4D7E-B469-3A81BECB2CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="2235" windowWidth="21600" windowHeight="11295" xr2:uid="{DC387A1A-0365-4EFE-8541-627FD66421E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DC387A1A-0365-4EFE-8541-627FD66421E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha4" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
   <si>
     <t>OPERAÇÃO</t>
   </si>
@@ -291,13 +291,16 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +333,14 @@
       <color indexed="56"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -396,11 +407,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,9 +435,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Folha Novembro 2010" xfId="1" xr:uid="{06716974-72D7-4BC5-BB3A-6BC3A896AA75}"/>
   </cellStyles>
@@ -731,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C5622E-29A2-43BB-87B8-5D1BD5310F6A}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,6 +803,9 @@
       <c r="F2" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="H2" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -818,7 +837,7 @@
       <c r="C4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3">
@@ -984,7 +1003,7 @@
       <c r="C12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="3">
@@ -1113,6 +1132,9 @@
       <c r="F18" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="H18" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -1133,6 +1155,9 @@
       <c r="F19" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="H19" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1210,7 +1235,7 @@
       <c r="C23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="3">
@@ -1219,6 +1244,9 @@
       <c r="F23" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="H23" s="9" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1281,6 +1309,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D23" r:id="rId1" xr:uid="{637C8505-8BF2-42A3-9079-B16B29588BD3}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>